<commit_message>
Added quality profiles for Dremel Nylon filament (temp for Draft 0.34 is now taken from quality profile). Ultra 0.05 quality is *not* available for selection!
</commit_message>
<xml_diff>
--- a/Dremel Digilab Slicer - Setting Comparison.xlsx
+++ b/Dremel Digilab Slicer - Setting Comparison.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="0.05" sheetId="3" r:id="rId1"/>
-    <sheet name="0.1" sheetId="1" r:id="rId2"/>
-    <sheet name="0.2" sheetId="2" r:id="rId3"/>
-    <sheet name="0.3" sheetId="4" r:id="rId4"/>
-    <sheet name="0.34" sheetId="5" r:id="rId5"/>
+    <sheet name="Ultra 0.05" sheetId="3" r:id="rId1"/>
+    <sheet name="High 0.1" sheetId="1" r:id="rId2"/>
+    <sheet name="Normal 0.2" sheetId="2" r:id="rId3"/>
+    <sheet name="Fast 0.3" sheetId="4" r:id="rId4"/>
+    <sheet name="Draft 0.34" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -745,12 +745,13 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
     <col min="3" max="4" width="52.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -883,7 +884,7 @@
       <c r="A8" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -4373,8 +4374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5552,8 +5553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>